<commit_message>
Change swt/LED pinouts to accept interrupts, add ISRs to code
</commit_message>
<xml_diff>
--- a/PCB-shield/REV2-BOM-prototype-cyc1.xlsx
+++ b/PCB-shield/REV2-BOM-prototype-cyc1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AOM\IoT-Bit\AoM-IoT-Bit\PCB-shield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B93D411-CE4B-480E-B72F-2D83AE6A5390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276137C3-A206-4CCB-A0C1-B37BFCFD32D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Name/Desc</t>
   </si>
@@ -161,6 +161,27 @@
   </si>
   <si>
     <t>www.digikey.com/en/products/detail/microchip-technology/VP0104N3-G/4902409</t>
+  </si>
+  <si>
+    <t>SH JST substitute test housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE </t>
+  </si>
+  <si>
+    <t>1470364-3</t>
+  </si>
+  <si>
+    <t>ZH JST test housing</t>
+  </si>
+  <si>
+    <t>ZHR-3</t>
+  </si>
+  <si>
+    <t>www.digikey.com/en/products/detail/te-connectivity-amp-connectors/1470364-3/2077839</t>
+  </si>
+  <si>
+    <t>www.digikey.com/en/products/detail/jst-sales-america-inc/ZHR-3/608602</t>
   </si>
 </sst>
 </file>
@@ -597,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,7 +695,7 @@
       </c>
       <c r="J2" s="13">
         <f>SUM(H1:H94)</f>
-        <v>6.6400000000000006</v>
+        <v>7.17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -697,7 +718,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H12" si="0">PRODUCT(E3*F3)</f>
+        <f t="shared" ref="H3:H16" si="0">PRODUCT(E3*F3)</f>
         <v>0.19</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -951,6 +972,60 @@
       <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>1.07</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -966,8 +1041,10 @@
     <hyperlink ref="G10" r:id="rId9" xr:uid="{7C11AB30-81AC-4B5E-9791-F1A37014A24A}"/>
     <hyperlink ref="G11" r:id="rId10" xr:uid="{25E7F621-5E13-4A79-8967-7EDFF40ACD54}"/>
     <hyperlink ref="G12" r:id="rId11" xr:uid="{DF70C0FA-A5D2-4AFA-99AC-2CD35B177167}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{69FD8A69-7DC6-49A4-A740-5F8A0604D722}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{C38E5E3C-BA0E-459E-9489-D48038303636}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>